<commit_message>
aufgabe 1 d + e
</commit_message>
<xml_diff>
--- a/Labor 1/Messwerte_Vorgabe.xlsx
+++ b/Labor 1/Messwerte_Vorgabe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuec\Desktop\Studium\SS 18\GLET\Labor\Labor 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nhuec\Desktop\Studium\SS 18\GLET\Labor\GLET-Service-\Labor 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2962F30-FFD0-4E6E-A2C6-745792FE9AA0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1876BB2C-4F50-42A4-A244-D906BC3431CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7100" xr2:uid="{E64AE6AF-014C-4B54-9F9A-21E6B5CC9842}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Temperatur </t>
   </si>
@@ -59,6 +58,40 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">𝛀 Approximiert mit </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Brückenspannung </t>
+  </si>
+  <si>
+    <r>
+      <t>R1 = R3 = 5100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria Math"/>
+        <family val="1"/>
+      </rPr>
+      <t>𝛀</t>
+    </r>
+  </si>
+  <si>
+    <t>U = 5V</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R4 = 100 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria Math"/>
+        <family val="1"/>
+      </rPr>
+      <t>𝛀</t>
     </r>
   </si>
 </sst>
@@ -239,841 +272,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Kennlinien Pt100</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12480835560322905"/>
-          <c:y val="0.14992091772199792"/>
-          <c:w val="0.83929527559055117"/>
-          <c:h val="0.61498432487605714"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$82</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.000</c:formatCode>
-                <c:ptCount val="81"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.39100000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.78100000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>101.172</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>101.562</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>101.953</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>102.343</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>102.733</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>103.123</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>103.51300000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>103.90300000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>104.292</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>104.682</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>105.071</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>105.46</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>105.849</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>106.238</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>106.627</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>107.01600000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>107.405</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>107.794</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>108.182</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>108.57</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>108.959</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>109.34699999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>109.735</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>110.123</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>110.51</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>110.898</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>111.286</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>111.673</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>112.06</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>112.447</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>112.83499999999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>113.221</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>113.608</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>113.995</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>114.38200000000001</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>114.768</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>115.155</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>115.541</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>115.92700000000001</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>116.313</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>116.699</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>117.08499999999999</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>117.47</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>117.85599999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>118.241</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>118.627</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>119.012</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>119.39700000000001</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>119.782</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>120.167</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>120.55200000000001</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>120.93600000000001</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>121.321</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>121.705</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>122.09</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>122.474</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>122.858</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>123.242</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>123.626</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>124.009</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>124.393</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>124.777</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>125.16</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>125.54300000000001</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>125.926</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>126.309</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>126.69199999999999</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>127.075</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>127.458</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>127.84</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>128.22300000000001</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>128.60499999999999</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>128.98699999999999</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>129.37</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>129.75200000000001</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>130.13300000000001</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>130.51499999999999</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>130.89699999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F792-4DA8-A899-CF073DDA5238}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="12700" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$C$2:$C$82</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="81"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100.3862125</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100.77242500000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>101.1586375</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>101.54485</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>101.9310625</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>102.31727500000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>102.70348749999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>103.08969999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>103.47591249999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>103.86212500000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>104.24833750000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>104.63454999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>105.0207625</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>105.406975</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>105.7931875</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>106.17939999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>106.5656125</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>106.951825</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>107.3380375</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>107.72425000000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>108.11046250000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>108.496675</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>108.8828875</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>109.26910000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>109.65531250000001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>110.04152499999999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>110.42773750000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>110.81395000000001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>111.2001625</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>111.58637499999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>111.9725875</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>112.3588</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>112.7450125</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>113.13122499999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>113.5174375</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>113.90365</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>114.2898625</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>114.67607499999998</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>115.06228750000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>115.4485</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>115.83471249999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>116.22092500000001</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>116.60713750000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>116.99334999999999</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>117.37956249999999</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>117.765775</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>118.1519875</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>118.53819999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>118.92441250000002</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>119.310625</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>119.6968375</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>120.08304999999999</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>120.46926250000001</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>120.855475</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>121.2416875</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>121.62790000000001</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>122.01411250000001</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>122.400325</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>122.78653749999999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>123.17275000000001</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>123.55896250000001</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>123.94517499999999</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>124.33138750000001</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>124.7176</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>125.1038125</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>125.49002499999999</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>125.87623749999999</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>126.26245</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>126.6486625</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>127.03487500000001</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>127.42108750000001</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>127.8073</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>128.1935125</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>128.579725</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>128.9659375</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>129.35214999999999</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>129.73836249999999</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>130.12457500000002</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>130.51078749999999</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>130.89699999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F792-4DA8-A899-CF073DDA5238}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="439440032"/>
-        <c:axId val="350918064"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="439440032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="350918064"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="350918064"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="90"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="439440032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
               <a:t>Fehlerdiagramm</a:t>
             </a:r>
           </a:p>
@@ -1553,6 +751,510 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11137510936132983"/>
+          <c:y val="0.11802092446777486"/>
+          <c:w val="0.86462860892388449"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$2:$E$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="81"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6870378518683022E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3640936739172158E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1050024287417859E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4725975951657144E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8410799825491209E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2085647829178656E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5759944895231701E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9433691147523477E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3106886709921568E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6779531706226942E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0442211336927381E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4113756983243935E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7775340328981564E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.1436376420144203E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5096865379394844E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.8756807329385374E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.2416202392717723E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.6075050691954962E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9733352349643507E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.3391107488268714E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.7038915365795768E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.068617977383119E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.4342298897543966E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.7988475330974536E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.1634108659444102E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.5279199004288939E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.8914354020862572E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0255836016098141E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0620182368096254E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0983535642747344E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.1346834958804175E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.1710080328283801E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2074210172509647E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.2436409275570215E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.2799492877396679E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.3162522580684177E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.3525498397434776E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.3887482626264158E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4250350845091964E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.4612227777889841E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.4974051149930778E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.5335820973106928E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5697537259303784E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.6059200020406283E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.6419872525897383E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6781428411032362E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7141994341063893E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7503443397601237E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.7863902799403752E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.8224309023849306E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.8584662082704595E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.8944961987732434E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.9305208750692304E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.9664466884275478E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.0024607536321404E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.038375985798313E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.0743794445990393E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.1102841002471062E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.146183476261776E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.1820775738074505E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.2179663940483096E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.2537564982696434E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.2896347811270923E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.3255077901668253E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.3612821278347074E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.3970512214269157E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.4328150720966391E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.4685736809962333E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.504327049278221E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.5400751780945141E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5758180685967469E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.6114624189546021E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.6471948499518505E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.6828287704037113E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.7184574844331677E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.7541742416096193E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.7897925325948703E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.8253123993948748E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.8609202991410343E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.8965229981661733E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B741-4B83-B1D7-17D6F0566CB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="338814736"/>
+        <c:axId val="338810800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="338814736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="338810800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="338810800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="338814736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2667,42 +2369,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>177188</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>86387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>569768</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>166831</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagramm 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BD78DE-A58A-4B72-A072-6B36F37E3659}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -2839,7 +2505,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2949,6 +2615,42 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>758825</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{519FBE15-EBD4-4CDD-896C-2AF45F2A08E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3311,19 +3013,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3E94F4-9B09-4DCE-ACB5-9F5341C63372}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="186" thickBot="1" x14ac:dyDescent="5.15">
+    <row r="1" spans="1:8" ht="186" thickBot="1" x14ac:dyDescent="5.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3336,8 +3040,20 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3351,8 +3067,12 @@
       <c r="D2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E2">
+        <f>5*(5100/(5100+100)-5100/(5100+B2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3367,8 +3087,12 @@
         <f t="shared" ref="D3:D66" si="0">B3-C3</f>
         <v>4.7875000000061618E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="1">5*(5100/(5100+100)-5100/(5100+B3))</f>
+        <v>3.6870378518683022E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3376,15 +3100,19 @@
         <v>100.78100000000001</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C67" si="1">100*(1+A4*0.003862125)</f>
+        <f t="shared" ref="C4:C67" si="2">100*(1+A4*0.003862125)</f>
         <v>100.77242500000001</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>8.574999999993338E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>7.3640936739172158E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3392,15 +3120,19 @@
         <v>101.172</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101.1586375</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>1.33624999999995E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1.1050024287417859E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3408,15 +3140,19 @@
         <v>101.562</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101.54485</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>1.7150000000000887E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1.4725975951657144E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3424,15 +3160,19 @@
         <v>101.953</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>101.9310625</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>2.1937500000007049E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1.8410799825491209E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3440,15 +3180,19 @@
         <v>102.343</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102.31727500000001</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
         <v>2.5724999999994225E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2.2085647829178656E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3456,15 +3200,19 @@
         <v>102.733</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102.70348749999999</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>2.9512500000009823E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2.5759944895231701E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3472,15 +3220,19 @@
         <v>103.123</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103.08969999999999</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>3.330000000001121E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2.9433691147523477E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3488,15 +3240,19 @@
         <v>103.51300000000001</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103.47591249999999</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>3.7087500000012597E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>3.3106886709921568E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3504,15 +3260,19 @@
         <v>103.90300000000001</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103.86212500000001</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>4.0874999999999773E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>3.6779531706226942E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3520,15 +3280,19 @@
         <v>104.292</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104.24833750000001</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>4.3662499999996385E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>4.0442211336927381E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3536,15 +3300,19 @@
         <v>104.682</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104.63454999999999</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>4.7450000000011983E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>4.4113756983243935E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3552,15 +3320,19 @@
         <v>105.071</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105.0207625</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>5.0237499999994384E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>4.7775340328981564E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3568,15 +3340,19 @@
         <v>105.46</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105.406975</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>5.3024999999990996E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>5.1436376420144203E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3584,15 +3360,19 @@
         <v>105.849</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105.7931875</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="0"/>
         <v>5.5812500000001819E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>5.5096865379394844E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3600,15 +3380,19 @@
         <v>106.238</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106.17939999999999</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="0"/>
         <v>5.8600000000012642E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>5.8756807329385374E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3616,15 +3400,19 @@
         <v>106.627</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106.5656125</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="0"/>
         <v>6.1387499999995043E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>6.2416202392717723E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3632,15 +3420,19 @@
         <v>107.01600000000001</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106.951825</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="0"/>
         <v>6.4175000000005866E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>6.6075050691954962E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3648,15 +3440,19 @@
         <v>107.405</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107.3380375</v>
       </c>
       <c r="D21" s="5">
         <f t="shared" si="0"/>
         <v>6.6962500000002478E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>6.9733352349643507E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3664,15 +3460,19 @@
         <v>107.794</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107.72425000000001</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="0"/>
         <v>6.974999999998488E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>7.3391107488268714E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3680,15 +3480,19 @@
         <v>108.182</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108.11046250000001</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="0"/>
         <v>7.1537499999990928E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>7.7038915365795768E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3696,15 +3500,19 @@
         <v>108.57</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108.496675</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="0"/>
         <v>7.3324999999996976E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>8.068617977383119E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3712,15 +3520,19 @@
         <v>108.959</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108.8828875</v>
       </c>
       <c r="D25" s="5">
         <f t="shared" si="0"/>
         <v>7.6112500000007799E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>8.4342298897543966E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3728,15 +3540,19 @@
         <v>109.34699999999999</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109.26910000000001</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" si="0"/>
         <v>7.7899999999985425E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>8.7988475330974536E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3744,15 +3560,19 @@
         <v>109.735</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109.65531250000001</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="0"/>
         <v>7.9687499999991473E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>9.1634108659444102E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3760,15 +3580,19 @@
         <v>110.123</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.04152499999999</v>
       </c>
       <c r="D28" s="5">
         <f t="shared" si="0"/>
         <v>8.1475000000011732E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>9.5279199004288939E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3776,15 +3600,19 @@
         <v>110.51</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.42773750000001</v>
       </c>
       <c r="D29" s="5">
         <f t="shared" si="0"/>
         <v>8.2262499999998795E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>9.8914354020862572E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3792,15 +3620,19 @@
         <v>110.898</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.81395000000001</v>
       </c>
       <c r="D30" s="5">
         <f t="shared" si="0"/>
         <v>8.4049999999990632E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>1.0255836016098141E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3808,15 +3640,19 @@
         <v>111.286</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111.2001625</v>
       </c>
       <c r="D31" s="5">
         <f t="shared" si="0"/>
         <v>8.583749999999668E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1.0620182368096254E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3824,15 +3660,19 @@
         <v>111.673</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111.58637499999999</v>
       </c>
       <c r="D32" s="5">
         <f t="shared" si="0"/>
         <v>8.6625000000012164E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>1.0983535642747344E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3840,15 +3680,19 @@
         <v>112.06</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111.9725875</v>
       </c>
       <c r="D33" s="5">
         <f t="shared" si="0"/>
         <v>8.7412499999999227E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>1.1346834958804175E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3856,15 +3700,19 @@
         <v>112.447</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112.3588</v>
       </c>
       <c r="D34" s="5">
         <f t="shared" si="0"/>
         <v>8.82000000000005E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>1.1710080328283801E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3872,15 +3720,19 @@
         <v>112.83499999999999</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112.7450125</v>
       </c>
       <c r="D35" s="5">
         <f t="shared" si="0"/>
         <v>8.9987499999992338E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>1.2074210172509647E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3888,15 +3740,19 @@
         <v>113.221</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.13122499999999</v>
       </c>
       <c r="D36" s="5">
         <f t="shared" si="0"/>
         <v>8.9775000000017258E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>1.2436409275570215E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3904,15 +3760,19 @@
         <v>113.608</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.5174375</v>
       </c>
       <c r="D37" s="5">
         <f t="shared" si="0"/>
         <v>9.056250000000432E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>1.2799492877396679E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3920,15 +3780,19 @@
         <v>113.995</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.90365</v>
       </c>
       <c r="D38" s="5">
         <f t="shared" si="0"/>
         <v>9.1350000000005593E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>1.3162522580684177E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3936,15 +3800,19 @@
         <v>114.38200000000001</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114.2898625</v>
       </c>
       <c r="D39" s="5">
         <f t="shared" si="0"/>
         <v>9.2137500000006867E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>1.3525498397434776E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3952,15 +3820,19 @@
         <v>114.768</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114.67607499999998</v>
       </c>
       <c r="D40" s="5">
         <f t="shared" si="0"/>
         <v>9.1925000000017576E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1.3887482626264158E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3968,15 +3840,19 @@
         <v>115.155</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.06228750000001</v>
       </c>
       <c r="D41" s="5">
         <f t="shared" si="0"/>
         <v>9.2712499999990428E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>1.4250350845091964E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3984,15 +3860,19 @@
         <v>115.541</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.4485</v>
       </c>
       <c r="D42" s="5">
         <f t="shared" si="0"/>
         <v>9.2500000000001137E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1.4612227777889841E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4000,15 +3880,19 @@
         <v>115.92700000000001</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115.83471249999999</v>
       </c>
       <c r="D43" s="5">
         <f t="shared" si="0"/>
         <v>9.2287500000011846E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>1.4974051149930778E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4016,15 +3900,19 @@
         <v>116.313</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116.22092500000001</v>
       </c>
       <c r="D44" s="5">
         <f t="shared" si="0"/>
         <v>9.2074999999994134E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>1.5335820973106928E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4032,15 +3920,19 @@
         <v>116.699</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116.60713750000001</v>
       </c>
       <c r="D45" s="5">
         <f t="shared" si="0"/>
         <v>9.1862499999990632E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>1.5697537259303784E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4048,15 +3940,19 @@
         <v>117.08499999999999</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116.99334999999999</v>
       </c>
       <c r="D46" s="5">
         <f t="shared" si="0"/>
         <v>9.1650000000001342E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1.6059200020406283E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4064,15 +3960,19 @@
         <v>117.47</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117.37956249999999</v>
       </c>
       <c r="D47" s="5">
         <f t="shared" si="0"/>
         <v>9.0437500000007276E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>1.6419872525897383E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4080,15 +3980,19 @@
         <v>117.85599999999999</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117.765775</v>
       </c>
       <c r="D48" s="5">
         <f t="shared" si="0"/>
         <v>9.0224999999989564E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>1.6781428411032362E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4096,15 +4000,19 @@
         <v>118.241</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.1519875</v>
       </c>
       <c r="D49" s="5">
         <f t="shared" si="0"/>
         <v>8.9012499999995498E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>1.7141994341063893E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4112,15 +4020,19 @@
         <v>118.627</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.53819999999999</v>
       </c>
       <c r="D50" s="5">
         <f t="shared" si="0"/>
         <v>8.8800000000006207E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>1.7503443397601237E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4128,15 +4040,19 @@
         <v>119.012</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118.92441250000002</v>
       </c>
       <c r="D51" s="5">
         <f t="shared" si="0"/>
         <v>8.758749999998372E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>1.7863902799403752E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4144,15 +4060,19 @@
         <v>119.39700000000001</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.310625</v>
       </c>
       <c r="D52" s="5">
         <f t="shared" si="0"/>
         <v>8.6375000000003865E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>1.8224309023849306E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4160,15 +4080,19 @@
         <v>119.782</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.6968375</v>
       </c>
       <c r="D53" s="5">
         <f t="shared" si="0"/>
         <v>8.5162499999995589E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>1.8584662082704595E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4176,15 +4100,19 @@
         <v>120.167</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.08304999999999</v>
       </c>
       <c r="D54" s="5">
         <f t="shared" si="0"/>
         <v>8.3950000000015734E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>1.8944961987732434E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4192,15 +4120,19 @@
         <v>120.55200000000001</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.46926250000001</v>
       </c>
       <c r="D55" s="5">
         <f t="shared" si="0"/>
         <v>8.2737499999993247E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>1.9305208750692304E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4208,15 +4140,19 @@
         <v>120.93600000000001</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.855475</v>
       </c>
       <c r="D56" s="5">
         <f t="shared" si="0"/>
         <v>8.0525000000008617E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>1.9664466884275478E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4224,15 +4160,19 @@
         <v>121.321</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121.2416875</v>
       </c>
       <c r="D57" s="5">
         <f t="shared" si="0"/>
         <v>7.9312500000000341E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>2.0024607536321404E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4240,15 +4180,19 @@
         <v>121.705</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121.62790000000001</v>
       </c>
       <c r="D58" s="5">
         <f t="shared" si="0"/>
         <v>7.709999999998729E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>2.038375985798313E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4256,15 +4200,19 @@
         <v>122.09</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122.01411250000001</v>
       </c>
       <c r="D59" s="5">
         <f t="shared" si="0"/>
         <v>7.5887499999993224E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>2.0743794445990393E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4272,15 +4220,19 @@
         <v>122.474</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122.400325</v>
       </c>
       <c r="D60" s="5">
         <f t="shared" si="0"/>
         <v>7.3675000000008595E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>2.1102841002471062E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4288,15 +4240,19 @@
         <v>122.858</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122.78653749999999</v>
       </c>
       <c r="D61" s="5">
         <f t="shared" si="0"/>
         <v>7.1462500000009754E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>2.146183476261776E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4304,15 +4260,19 @@
         <v>123.242</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.17275000000001</v>
       </c>
       <c r="D62" s="5">
         <f t="shared" si="0"/>
         <v>6.9249999999996703E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>2.1820775738074505E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4320,15 +4280,19 @@
         <v>123.626</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.55896250000001</v>
       </c>
       <c r="D63" s="5">
         <f t="shared" si="0"/>
         <v>6.7037499999997863E-2</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>2.2179663940483096E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4336,15 +4300,19 @@
         <v>124.009</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123.94517499999999</v>
       </c>
       <c r="D64" s="5">
         <f t="shared" si="0"/>
         <v>6.3825000000008458E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>2.2537564982696434E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4352,15 +4320,19 @@
         <v>124.393</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.33138750000001</v>
       </c>
       <c r="D65" s="5">
         <f t="shared" si="0"/>
         <v>6.1612499999995407E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>2.2896347811270923E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4368,15 +4340,19 @@
         <v>124.777</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.7176</v>
       </c>
       <c r="D66" s="5">
         <f t="shared" si="0"/>
         <v>5.9399999999996567E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>2.3255077901668253E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4384,15 +4360,19 @@
         <v>125.16</v>
       </c>
       <c r="C67" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>125.1038125</v>
       </c>
       <c r="D67" s="5">
-        <f t="shared" ref="D67:D82" si="2">B67-C67</f>
+        <f t="shared" ref="D67:D82" si="3">B67-C67</f>
         <v>5.6187499999992951E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E67">
+        <f t="shared" ref="E67:E82" si="4">5*(5100/(5100+100)-5100/(5100+B67))</f>
+        <v>2.3612821278347074E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4400,15 +4380,19 @@
         <v>125.54300000000001</v>
       </c>
       <c r="C68" s="1">
-        <f t="shared" ref="C68:C82" si="3">100*(1+A68*0.003862125)</f>
+        <f t="shared" ref="C68:C82" si="5">100*(1+A68*0.003862125)</f>
         <v>125.49002499999999</v>
       </c>
       <c r="D68" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.2975000000017758E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E68">
+        <f t="shared" si="4"/>
+        <v>2.3970512214269157E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4416,15 +4400,19 @@
         <v>125.926</v>
       </c>
       <c r="C69" s="1">
+        <f t="shared" si="5"/>
+        <v>125.87623749999999</v>
+      </c>
+      <c r="D69" s="5">
         <f t="shared" si="3"/>
-        <v>125.87623749999999</v>
-      </c>
-      <c r="D69" s="5">
-        <f t="shared" si="2"/>
         <v>4.9762500000014143E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E69">
+        <f t="shared" si="4"/>
+        <v>2.4328150720966391E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4432,15 +4420,19 @@
         <v>126.309</v>
       </c>
       <c r="C70" s="1">
+        <f t="shared" si="5"/>
+        <v>126.26245</v>
+      </c>
+      <c r="D70" s="5">
         <f t="shared" si="3"/>
-        <v>126.26245</v>
-      </c>
-      <c r="D70" s="5">
-        <f t="shared" si="2"/>
         <v>4.6549999999996317E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E70">
+        <f t="shared" si="4"/>
+        <v>2.4685736809962333E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4448,15 +4440,19 @@
         <v>126.69199999999999</v>
       </c>
       <c r="C71" s="1">
+        <f t="shared" si="5"/>
+        <v>126.6486625</v>
+      </c>
+      <c r="D71" s="5">
         <f t="shared" si="3"/>
-        <v>126.6486625</v>
-      </c>
-      <c r="D71" s="5">
-        <f t="shared" si="2"/>
         <v>4.3337499999992701E-2</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E71">
+        <f t="shared" si="4"/>
+        <v>2.504327049278221E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4464,15 +4460,19 @@
         <v>127.075</v>
       </c>
       <c r="C72" s="1">
+        <f t="shared" si="5"/>
+        <v>127.03487500000001</v>
+      </c>
+      <c r="D72" s="5">
         <f t="shared" si="3"/>
-        <v>127.03487500000001</v>
-      </c>
-      <c r="D72" s="5">
-        <f t="shared" si="2"/>
         <v>4.0124999999989086E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E72">
+        <f t="shared" si="4"/>
+        <v>2.5400751780945141E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4480,15 +4480,19 @@
         <v>127.458</v>
       </c>
       <c r="C73" s="1">
+        <f t="shared" si="5"/>
+        <v>127.42108750000001</v>
+      </c>
+      <c r="D73" s="5">
         <f t="shared" si="3"/>
-        <v>127.42108750000001</v>
-      </c>
-      <c r="D73" s="5">
-        <f t="shared" si="2"/>
         <v>3.6912499999985471E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E73">
+        <f t="shared" si="4"/>
+        <v>2.5758180685967469E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4496,15 +4500,19 @@
         <v>127.84</v>
       </c>
       <c r="C74" s="1">
+        <f t="shared" si="5"/>
+        <v>127.8073</v>
+      </c>
+      <c r="D74" s="5">
         <f t="shared" si="3"/>
-        <v>127.8073</v>
-      </c>
-      <c r="D74" s="5">
-        <f t="shared" si="2"/>
         <v>3.2700000000005502E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E74">
+        <f t="shared" si="4"/>
+        <v>2.6114624189546021E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4512,15 +4520,19 @@
         <v>128.22300000000001</v>
       </c>
       <c r="C75" s="1">
+        <f t="shared" si="5"/>
+        <v>128.1935125</v>
+      </c>
+      <c r="D75" s="5">
         <f t="shared" si="3"/>
-        <v>128.1935125</v>
-      </c>
-      <c r="D75" s="5">
-        <f t="shared" si="2"/>
         <v>2.9487500000016098E-2</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E75">
+        <f t="shared" si="4"/>
+        <v>2.6471948499518505E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4528,15 +4540,19 @@
         <v>128.60499999999999</v>
       </c>
       <c r="C76" s="1">
+        <f t="shared" si="5"/>
+        <v>128.579725</v>
+      </c>
+      <c r="D76" s="5">
         <f t="shared" si="3"/>
-        <v>128.579725</v>
-      </c>
-      <c r="D76" s="5">
-        <f t="shared" si="2"/>
         <v>2.5274999999993497E-2</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E76">
+        <f t="shared" si="4"/>
+        <v>2.6828287704037113E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4544,15 +4560,19 @@
         <v>128.98699999999999</v>
       </c>
       <c r="C77" s="1">
+        <f t="shared" si="5"/>
+        <v>128.9659375</v>
+      </c>
+      <c r="D77" s="5">
         <f t="shared" si="3"/>
-        <v>128.9659375</v>
-      </c>
-      <c r="D77" s="5">
-        <f t="shared" si="2"/>
         <v>2.1062499999999318E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E77">
+        <f t="shared" si="4"/>
+        <v>2.7184574844331677E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4560,15 +4580,19 @@
         <v>129.37</v>
       </c>
       <c r="C78" s="1">
+        <f t="shared" si="5"/>
+        <v>129.35214999999999</v>
+      </c>
+      <c r="D78" s="5">
         <f t="shared" si="3"/>
-        <v>129.35214999999999</v>
-      </c>
-      <c r="D78" s="5">
-        <f t="shared" si="2"/>
         <v>1.7850000000009913E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E78">
+        <f t="shared" si="4"/>
+        <v>2.7541742416096193E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4576,15 +4600,19 @@
         <v>129.75200000000001</v>
       </c>
       <c r="C79" s="1">
+        <f t="shared" si="5"/>
+        <v>129.73836249999999</v>
+      </c>
+      <c r="D79" s="5">
         <f t="shared" si="3"/>
-        <v>129.73836249999999</v>
-      </c>
-      <c r="D79" s="5">
-        <f t="shared" si="2"/>
         <v>1.3637500000015734E-2</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E79">
+        <f t="shared" si="4"/>
+        <v>2.7897925325948703E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>78</v>
       </c>
@@ -4592,15 +4620,19 @@
         <v>130.13300000000001</v>
       </c>
       <c r="C80" s="1">
+        <f t="shared" si="5"/>
+        <v>130.12457500000002</v>
+      </c>
+      <c r="D80" s="5">
         <f t="shared" si="3"/>
-        <v>130.12457500000002</v>
-      </c>
-      <c r="D80" s="5">
-        <f t="shared" si="2"/>
         <v>8.4249999999883585E-3</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E80">
+        <f t="shared" si="4"/>
+        <v>2.8253123993948748E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>79</v>
       </c>
@@ -4608,15 +4640,19 @@
         <v>130.51499999999999</v>
       </c>
       <c r="C81" s="1">
+        <f t="shared" si="5"/>
+        <v>130.51078749999999</v>
+      </c>
+      <c r="D81" s="5">
         <f t="shared" si="3"/>
-        <v>130.51078749999999</v>
-      </c>
-      <c r="D81" s="5">
-        <f t="shared" si="2"/>
         <v>4.2124999999941792E-3</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E81">
+        <f t="shared" si="4"/>
+        <v>2.8609202991410343E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>80</v>
       </c>
@@ -4624,54 +4660,58 @@
         <v>130.89699999999999</v>
       </c>
       <c r="C82" s="1">
+        <f t="shared" si="5"/>
+        <v>130.89699999999999</v>
+      </c>
+      <c r="D82" s="5">
         <f t="shared" si="3"/>
-        <v>130.89699999999999</v>
-      </c>
-      <c r="D82" s="5">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E82">
+        <f t="shared" si="4"/>
+        <v>2.8965229981661733E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B84" s="7"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B85" s="7"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B86" s="7"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B87" s="7"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B88" s="7"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B89" s="7"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B90" s="7"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B91" s="7"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B92" s="7"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B93" s="7"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B94" s="7"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B95" s="7"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B96" s="7"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">

</xml_diff>